<commit_message>
small changes in all notebooks..
</commit_message>
<xml_diff>
--- a/input/transport_stats/wege_zweck_poiskeys.xlsx
+++ b/input/transport_stats/wege_zweck_poiskeys.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t xml:space="preserve">Ziel/Zweck</t>
   </si>
@@ -34,30 +34,48 @@
     <t xml:space="preserve">AlleWege</t>
   </si>
   <si>
+    <t xml:space="preserve">Wegzweck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km_Wegzweck</t>
+  </si>
+  <si>
     <t xml:space="preserve">POI-keys</t>
   </si>
   <si>
     <t xml:space="preserve">Summe Schule</t>
   </si>
   <si>
+    <t xml:space="preserve">Ausbildung;Begleitung</t>
+  </si>
+  <si>
     <t xml:space="preserve">kindergarten;school;university;college</t>
   </si>
   <si>
     <t xml:space="preserve">Summe Einkauf</t>
   </si>
   <si>
+    <t xml:space="preserve">Einkauf</t>
+  </si>
+  <si>
     <t xml:space="preserve">pharmacy;marketplace;retail;hardware;garden_centre;supermarket;convenience;butcher;beverages;clothes;doityourself;shoes;mall;greengrocer;department_store;bakery;electronics;winery</t>
   </si>
   <si>
     <t xml:space="preserve">Eigener Arbeitsplatz</t>
   </si>
   <si>
+    <t xml:space="preserve">Arbeit</t>
+  </si>
+  <si>
     <t xml:space="preserve">Anderer Dienstort/-weg</t>
   </si>
   <si>
     <t xml:space="preserve">Behördengang. Arztbesuch</t>
   </si>
   <si>
+    <t xml:space="preserve">Erledigung</t>
+  </si>
+  <si>
     <t xml:space="preserve">doctors;clinic;hospital</t>
   </si>
   <si>
@@ -68,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">Kultur. Theater. Kino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freizeit</t>
   </si>
   <si>
     <t xml:space="preserve">cinema;arts_centre;theatre;nightclub;events_venue</t>
@@ -199,18 +220,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.74"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -226,14 +247,19 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>6.6</v>
@@ -244,13 +270,20 @@
       <c r="D2" s="0" t="n">
         <v>6.3</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>6</v>
+      <c r="E2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <f aca="false">(7+8)/2</f>
+        <v>7.5</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>11.4</v>
@@ -261,13 +294,19 @@
       <c r="D3" s="0" t="n">
         <v>11.2</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>8</v>
+      <c r="E3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>13.1</v>
@@ -278,10 +317,16 @@
       <c r="D4" s="0" t="n">
         <v>13.4</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2.1</v>
@@ -292,10 +337,16 @@
       <c r="D5" s="0" t="n">
         <v>2.5</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>3.2</v>
@@ -306,14 +357,20 @@
       <c r="D6" s="0" t="n">
         <v>3.1</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="1"/>
+      <c r="E6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2.5</v>
@@ -324,13 +381,19 @@
       <c r="D7" s="0" t="n">
         <v>2.4</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>14</v>
+      <c r="E7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.7</v>
@@ -341,13 +404,19 @@
       <c r="D8" s="0" t="n">
         <v>0.7</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>16</v>
+      <c r="E8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>3.1</v>
@@ -358,15 +427,21 @@
       <c r="D9" s="0" t="n">
         <v>3.2</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="E9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="K9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>8.7</v>
@@ -377,13 +452,19 @@
       <c r="D10" s="0" t="n">
         <v>8.9</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>20</v>
+      <c r="E10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>39.2</v>
@@ -394,10 +475,16 @@
       <c r="D11" s="0" t="n">
         <v>38.9</v>
       </c>
+      <c r="E11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>9.2</v>
@@ -411,7 +498,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>123899</v>
@@ -425,7 +512,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>124418</v>

</xml_diff>

<commit_message>
added bike mode. added scenario option for car free inner cities (need to be configured in exc3). moved prices to exc3.
</commit_message>
<xml_diff>
--- a/input/transport_stats/wege_zweck_poiskeys.xlsx
+++ b/input/transport_stats/wege_zweck_poiskeys.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Education</t>
   </si>
   <si>
-    <t xml:space="preserve">Education;accompaniment </t>
+    <t xml:space="preserve">Education;Accompaniment </t>
   </si>
   <si>
     <t xml:space="preserve">kindergarten;school;university;college</t>
@@ -274,10 +274,10 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>

</xml_diff>

<commit_message>
restructured notebook folder and renamed notebooks.
</commit_message>
<xml_diff>
--- a/input/transport_stats/wege_zweck_poiskeys.xlsx
+++ b/input/transport_stats/wege_zweck_poiskeys.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Education</t>
   </si>
   <si>
-    <t xml:space="preserve">Education;Accompaniment </t>
+    <t xml:space="preserve">Education;Accompaniment</t>
   </si>
   <si>
     <t xml:space="preserve">kindergarten;school;university;college</t>
@@ -274,10 +274,10 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>

</xml_diff>